<commit_message>
Add Create New Account feature file - Gherkin Test
</commit_message>
<xml_diff>
--- a/Data Files/createacc-invalidemail.xlsx
+++ b/Data Files/createacc-invalidemail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silmi\Katalon Studio\Magento - Web Automation Testing\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{752F2E75-D902-41C6-AF2B-51A5EA7504B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8240FCAE-17D2-4441-8B8A-2B0DC15BEBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5B91FF4-F66F-4C87-BBE0-D77E63DB20CB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>first_name</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>ABCde!12348</t>
+  </si>
+  <si>
+    <t>registered email</t>
+  </si>
+  <si>
+    <t>ABCde!12349</t>
+  </si>
+  <si>
+    <t>magento.silmi@test.com</t>
+  </si>
+  <si>
+    <t>Silmi</t>
+  </si>
+  <si>
+    <t>Fillah</t>
   </si>
 </sst>
 </file>
@@ -463,20 +478,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237EE355-367A-4C02-AA84-F3B2E9AEF382}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -579,10 +594,31 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{014F863A-A95F-40C7-9F1A-EF190421D6AC}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{51CD6F0C-31D1-40D5-A49B-FFDB6031D893}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>